<commit_message>
modified:   Programming Language Notes.xlsx
</commit_message>
<xml_diff>
--- a/Programming Language Notes.xlsx
+++ b/Programming Language Notes.xlsx
@@ -8,12 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\Development\Study Notes for Code Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8527A8-AD64-4C81-9B07-D57664156F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6CF51C-F163-41FD-A424-71BB95FA2F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="711" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId2"/>
+    <sheet name="Comment" sheetId="7" r:id="rId3"/>
+    <sheet name="Data Types" sheetId="2" r:id="rId4"/>
+    <sheet name="Operators" sheetId="6" r:id="rId5"/>
+    <sheet name="Expressions" sheetId="4" r:id="rId6"/>
+    <sheet name="Statements" sheetId="5" r:id="rId7"/>
+    <sheet name="Preprocessor" sheetId="8" r:id="rId8"/>
+    <sheet name="Function" sheetId="10" r:id="rId9"/>
+    <sheet name="Library" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,8 +33,80 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johnson Zhou</author>
+  </authors>
+  <commentList>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{0AE5F3B8-CA41-4F5F-8689-13F2A3FB13CB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>元组即不可修改元素的列表，但可以更改元组的定义</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johnson Zhou</author>
+  </authors>
+  <commentList>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{F6AFC271-CAED-4BF6-9B9C-E9C003A87A96}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>使用默认值时，在形参列表中必须先列出没有默认值的形参，再列出有默认值的实参。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{F5241F1B-1F2C-4C1E-A825-75EDFD847261}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>使用空元组</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{E329C447-546B-4919-B8CC-01FE525DB491}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>使用空字典</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="179">
   <si>
     <t>C</t>
   </si>
@@ -392,12 +473,410 @@
   <si>
     <t>跳转语句</t>
   </si>
+  <si>
+    <t>操控数据</t>
+  </si>
+  <si>
+    <t>floating-point</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>primitive types</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>#include &lt;….h&gt;</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>函数体开始与结束</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>函数头声明与调用操作符</t>
+  </si>
+  <si>
+    <t>stdio.h</t>
+  </si>
+  <si>
+    <t>标准输入输出</t>
+  </si>
+  <si>
+    <t>preprocessor directive</t>
+  </si>
+  <si>
+    <t>块开始与结束</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>命名</t>
+  </si>
+  <si>
+    <t>包含小写字母、大写字母、数字和下划线
+第一个字符不能是数字
+区分大小写</t>
+  </si>
+  <si>
+    <t>表达式语句
+* 赋值表达式语句</t>
+  </si>
+  <si>
+    <t>赋值运算符</t>
+  </si>
+  <si>
+    <t>占位符</t>
+  </si>
+  <si>
+    <t>标准IO</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>赋值表达式</t>
+  </si>
+  <si>
+    <t>函数调用表达式</t>
+  </si>
+  <si>
+    <t>声明函数原型</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>extern</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>goto</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>restrict</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>signed</t>
+  </si>
+  <si>
+    <t>sizeof</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>struct</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>typedef</t>
+  </si>
+  <si>
+    <t>union</t>
+  </si>
+  <si>
+    <t>unsigned</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>volatile</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>_Alignas</t>
+  </si>
+  <si>
+    <t>_Alignof</t>
+  </si>
+  <si>
+    <t>_Atomic</t>
+  </si>
+  <si>
+    <t>_Bool</t>
+  </si>
+  <si>
+    <t>_Complex</t>
+  </si>
+  <si>
+    <t>_Generic</t>
+  </si>
+  <si>
+    <t>_Imaginary</t>
+  </si>
+  <si>
+    <t>_Noreturn</t>
+  </si>
+  <si>
+    <t>_Static_assert</t>
+  </si>
+  <si>
+    <t>_Thread_local</t>
+  </si>
+  <si>
+    <t>十进制整数</t>
+  </si>
+  <si>
+    <t>浮点数</t>
+  </si>
+  <si>
+    <t>%f</t>
+  </si>
+  <si>
+    <t>十六进制整数</t>
+  </si>
+  <si>
+    <t>八进制整数</t>
+  </si>
+  <si>
+    <t>%o, %#o</t>
+  </si>
+  <si>
+    <t>_Bool, char, short, int, long, long long</t>
+  </si>
+  <si>
+    <t>%hhd, %hd, %d, %u, %ld, %lu, %ll, %llu</t>
+  </si>
+  <si>
+    <t>%hx, %x, , %#x, %X, %#X, %lx, %lX</t>
+  </si>
+  <si>
+    <t>换行符	\n
+水平制表符	\t
+垂直制表符	\v
+退格符	\b
+回车符	\r
+警报符	\a
+换页符	\f
+反斜杠	\\
+单引号	\'
+双引号	\"
+问号	\?
+八进制	\0oo
+十六进制	\xhh</t>
+  </si>
+  <si>
+    <t>复杂类型</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>换行符	\n
+水平制表符	\t</t>
+  </si>
+  <si>
+    <t>算数运算符</t>
+  </si>
+  <si>
+    <t>+,-,*,/,**</t>
+  </si>
+  <si>
+    <t>title(),lower(),upper(),拼接字符串+,strip(),rstrip(),lstrip(),str()</t>
+  </si>
+  <si>
+    <t>空列表[],倒数列表[-1],[-2],append(),insert(),del,pop(),remove(),sort(),sorted(),revers(),len(),for…in…,</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>return_type function_name(parameters)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>def</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function_name(parameters)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>定义函数头</t>
+  </si>
+  <si>
+    <t>定义函数体</t>
+  </si>
+  <si>
+    <t>{statements;}</t>
+  </si>
+  <si>
+    <t>indent statements</t>
+  </si>
+  <si>
+    <t>文档字符串</t>
+  </si>
+  <si>
+    <t>"""comment statements"""</t>
+  </si>
+  <si>
+    <t>函数调用</t>
+  </si>
+  <si>
+    <t>function_name(arguments)</t>
+  </si>
+  <si>
+    <t>实参</t>
+  </si>
+  <si>
+    <t>形参</t>
+  </si>
+  <si>
+    <t>关键字实参</t>
+  </si>
+  <si>
+    <t>默认值</t>
+  </si>
+  <si>
+    <t>positional arguments</t>
+  </si>
+  <si>
+    <t>返回值</t>
+  </si>
+  <si>
+    <t>让实参变成可选的</t>
+  </si>
+  <si>
+    <t>设置默认值为空字符串</t>
+  </si>
+  <si>
+    <t>禁止函数修改列表</t>
+  </si>
+  <si>
+    <t>切片表示法创建列表的副本function_name(list_name[:])</t>
+  </si>
+  <si>
+    <t>传递任意无限数量的实参</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>元组</t>
+  </si>
+  <si>
+    <t>tuple(1,2)</t>
+  </si>
+  <si>
+    <t>切片</t>
+  </si>
+  <si>
+    <t>[:]</t>
+  </si>
+  <si>
+    <t>结合使用位置实参和任意数量实参</t>
+  </si>
+  <si>
+    <t>function(parameter1,*tuple_parameter)</t>
+  </si>
+  <si>
+    <t>使用任意数量的关键字实参</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** </t>
+  </si>
+  <si>
+    <t>字典</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,16 +915,50 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -488,11 +1001,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -515,11 +1044,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -800,16 +1347,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -826,20 +1373,20 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B2" t="s">
@@ -850,7 +1397,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>48</v>
       </c>
@@ -860,13 +1407,13 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -901,12 +1448,12 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -918,11 +1465,11 @@
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -932,33 +1479,33 @@
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -968,7 +1515,7 @@
       <c r="D18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -982,11 +1529,11 @@
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>28</v>
       </c>
@@ -996,11 +1543,11 @@
       <c r="D20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>28</v>
       </c>
@@ -1008,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="H21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1020,7 +1567,7 @@
         <v>16</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="H22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="1"/>
@@ -1032,7 +1579,7 @@
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1044,7 +1591,7 @@
         <v>29</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="H24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1055,7 +1602,7 @@
       <c r="C25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1066,7 +1613,7 @@
       <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1077,7 +1624,7 @@
       <c r="C27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1088,12 +1635,12 @@
       <c r="C28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -1101,31 +1648,31 @@
       </c>
     </row>
     <row r="30" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="7" t="s">
         <v>61</v>
       </c>
@@ -1138,4 +1685,1024 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75BDFCC-E8CE-4DAD-8A87-4975946EFA77}">
+  <dimension ref="C1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57655670-389F-4B23-97FB-F7964371C7CE}">
+  <dimension ref="D1:H45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E80B5C9-D50D-4C88-A574-918199AB13F5}">
+  <dimension ref="C1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1E8EDA-3250-49E3-9FBB-405740BFCD0F}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A2:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52578695-A485-4669-889D-29C1B5978D9F}">
+  <dimension ref="C1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C603AC53-561E-40FC-9D91-EBDEE5587800}">
+  <dimension ref="C1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DFCDC4-611B-4152-88F4-2E2A064DC973}">
+  <dimension ref="C1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C83AF20-B752-4DDA-A01D-0340EEFA7964}">
+  <dimension ref="C1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A5F2E5-2C78-4131-9687-D551073ABA4E}">
+  <dimension ref="B1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+      <c r="C10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="11"/>
+      <c r="C14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B7:B14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>